<commit_message>
Editor with cell number
</commit_message>
<xml_diff>
--- a/resources/difficulty.xlsx
+++ b/resources/difficulty.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Level</t>
   </si>
@@ -50,19 +50,31 @@
     <t>Nb Shapes</t>
   </si>
   <si>
-    <t>ultra easy</t>
+    <t>12 shapes</t>
   </si>
   <si>
-    <t>easy</t>
+    <t>Normal</t>
   </si>
   <si>
-    <t>impossible</t>
+    <t>shapes</t>
   </si>
   <si>
-    <t>hard</t>
+    <t>nbcel</t>
   </si>
   <si>
-    <t>very hard</t>
+    <t>50/70</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Meidum</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Master</t>
   </si>
 </sst>
 </file>
@@ -414,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I191"/>
+  <dimension ref="B3:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -442,16 +454,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E16" si="0">D4*C4</f>
-        <v>9</v>
+        <f t="shared" ref="E4:E18" si="0">D4*C4</f>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -462,88 +477,109 @@
       </c>
       <c r="I4">
         <f>F4/E4</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H68" si="1">E5*POWER(F5,7)*I5</f>
-        <v>390625</v>
+        <v>65536</v>
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I18" si="2">F5/E5</f>
-        <v>0.1388888888888889</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
       <c r="C6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>16777216</v>
+        <v>390625</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>0.22222222222222221</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
       <c r="C7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="F7">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>16777216</v>
+        <v>1679616</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>8</v>
+      </c>
+      <c r="M7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
       <c r="C8">
         <v>6</v>
       </c>
@@ -555,303 +591,315 @@
         <v>36</v>
       </c>
       <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>100000000</v>
+        <v>5764801</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>0.27777777777777779</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
       <c r="C9">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>100000000</v>
+        <v>16777216</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>0.1388888888888889</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
       <c r="C10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>429981696</v>
+        <v>1679616</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.12244897959183673</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10">
+        <v>11</v>
+      </c>
+      <c r="M10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
       <c r="C11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>6561</v>
+        <v>5764801</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
       <c r="C12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>390625</v>
+        <v>16777215.999999998</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>6.9444444444444448E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.16326530612244897</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
       <c r="C13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="F13">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>429981696</v>
+        <v>43046721</v>
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
+        <v>0.18367346938775511</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>7</v>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="F15">
-        <v>12</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>429981696</v>
-      </c>
-      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" t="e">
         <f t="shared" si="2"/>
-        <v>0.24489795918367346</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>9</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" t="e">
         <f t="shared" si="2"/>
-        <v>1.3888888888888888E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E67" si="3">D17*C17</f>
-        <v>100</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" t="e">
         <f t="shared" si="2"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E17:E67" si="3">D19*C19</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>20</v>
       </c>
-      <c r="D18">
-        <v>20</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>400</v>
-      </c>
-      <c r="F18">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
-        <v>100000000</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E23">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -861,7 +909,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>21</v>
+      </c>
       <c r="E24">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -871,7 +922,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>22</v>
+      </c>
       <c r="E25">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -881,7 +935,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>23</v>
+      </c>
       <c r="E26">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -891,7 +948,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>24</v>
+      </c>
       <c r="E27">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -901,7 +961,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>25</v>
+      </c>
       <c r="E28">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -911,7 +974,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>26</v>
+      </c>
       <c r="E29">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -921,7 +987,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>27</v>
+      </c>
       <c r="E30">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -931,7 +1000,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>28</v>
+      </c>
       <c r="E31">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -941,7 +1013,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>29</v>
+      </c>
       <c r="E32">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -952,6 +1027,9 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>30</v>
+      </c>
       <c r="E33">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -962,6 +1040,9 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>31</v>
+      </c>
       <c r="E34">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -972,6 +1053,9 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>32</v>
+      </c>
       <c r="E35">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -982,6 +1066,9 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>33</v>
+      </c>
       <c r="E36">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -992,6 +1079,9 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>34</v>
+      </c>
       <c r="E37">
         <f t="shared" si="3"/>
         <v>0</v>

</xml_diff>